<commit_message>
Filled in as many missing salaries for pitchers that baseball-reference.com had.
</commit_message>
<xml_diff>
--- a/data/Baseball_pitchers_data.xlsx
+++ b/data/Baseball_pitchers_data.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Davis\15F\ECS171 Mach Learn\Proj\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22100" windowHeight="10030"/>
+    <workbookView xWindow="55500" yWindow="20" windowWidth="15340" windowHeight="20740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="252">
   <si>
     <t>name</t>
   </si>
@@ -877,7 +875,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -912,7 +910,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1089,7 +1087,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1099,31 +1097,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="Q194" sqref="Q194"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="14" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1408,8 +1408,8 @@
       <c r="P5">
         <v>3</v>
       </c>
-      <c r="Q5" t="s">
-        <v>24</v>
+      <c r="Q5">
+        <v>650</v>
       </c>
       <c r="R5" t="s">
         <v>22</v>
@@ -1418,7 +1418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1762,8 +1762,8 @@
       <c r="P11">
         <v>6</v>
       </c>
-      <c r="Q11" t="s">
-        <v>24</v>
+      <c r="Q11">
+        <v>75</v>
       </c>
       <c r="R11" t="s">
         <v>22</v>
@@ -1772,7 +1772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -2057,8 +2057,8 @@
       <c r="P16">
         <v>0</v>
       </c>
-      <c r="Q16" t="s">
-        <v>24</v>
+      <c r="Q16">
+        <v>110</v>
       </c>
       <c r="R16" t="s">
         <v>22</v>
@@ -2067,7 +2067,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -2352,8 +2352,8 @@
       <c r="P21">
         <v>10</v>
       </c>
-      <c r="Q21" t="s">
-        <v>24</v>
+      <c r="Q21">
+        <v>250</v>
       </c>
       <c r="R21" t="s">
         <v>20</v>
@@ -2362,7 +2362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -2411,8 +2411,8 @@
       <c r="P22">
         <v>0</v>
       </c>
-      <c r="Q22" t="s">
-        <v>24</v>
+      <c r="Q22">
+        <v>550</v>
       </c>
       <c r="R22" t="s">
         <v>20</v>
@@ -2421,7 +2421,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -2529,8 +2529,8 @@
       <c r="P24">
         <v>12</v>
       </c>
-      <c r="Q24" t="s">
-        <v>24</v>
+      <c r="Q24">
+        <v>210</v>
       </c>
       <c r="R24" t="s">
         <v>22</v>
@@ -2539,7 +2539,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -3178,8 +3178,8 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="Q35" t="s">
-        <v>24</v>
+      <c r="Q35">
+        <v>115</v>
       </c>
       <c r="R35" t="s">
         <v>22</v>
@@ -3188,7 +3188,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>102</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19">
       <c r="A58" t="s">
         <v>103</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>104</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
         <v>105</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19">
       <c r="A61" t="s">
         <v>106</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19">
       <c r="A62" t="s">
         <v>107</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19">
       <c r="A63" t="s">
         <v>108</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19">
       <c r="A64" t="s">
         <v>109</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19">
       <c r="A65" t="s">
         <v>110</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:19">
       <c r="A66" t="s">
         <v>111</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19">
       <c r="A67" t="s">
         <v>112</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:19">
       <c r="A68" t="s">
         <v>113</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:19">
       <c r="A69" t="s">
         <v>114</v>
       </c>
@@ -5184,8 +5184,8 @@
       <c r="P69">
         <v>4</v>
       </c>
-      <c r="Q69" t="s">
-        <v>24</v>
+      <c r="Q69">
+        <v>850</v>
       </c>
       <c r="R69" t="s">
         <v>20</v>
@@ -5194,7 +5194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:19">
       <c r="A70" t="s">
         <v>115</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:19">
       <c r="A71" t="s">
         <v>116</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:19">
       <c r="A72" t="s">
         <v>117</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:19">
       <c r="A73" t="s">
         <v>118</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:19">
       <c r="A74" t="s">
         <v>119</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:19">
       <c r="A75" t="s">
         <v>120</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:19">
       <c r="A76" t="s">
         <v>121</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:19">
       <c r="A77" t="s">
         <v>122</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:19">
       <c r="A78" t="s">
         <v>123</v>
       </c>
@@ -5715,8 +5715,8 @@
       <c r="P78">
         <v>1</v>
       </c>
-      <c r="Q78" t="s">
-        <v>24</v>
+      <c r="Q78">
+        <v>150</v>
       </c>
       <c r="R78" t="s">
         <v>22</v>
@@ -5725,7 +5725,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:19">
       <c r="A79" t="s">
         <v>124</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:19">
       <c r="A80" t="s">
         <v>125</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19">
       <c r="A81" t="s">
         <v>126</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:19">
       <c r="A82" t="s">
         <v>127</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:19">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:19">
       <c r="A84" t="s">
         <v>129</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19">
       <c r="A85" t="s">
         <v>130</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19">
       <c r="A86" t="s">
         <v>131</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:19">
       <c r="A87" t="s">
         <v>132</v>
       </c>
@@ -6256,7 +6256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:19">
       <c r="A88" t="s">
         <v>133</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:19">
       <c r="A89" t="s">
         <v>134</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19">
       <c r="A90" t="s">
         <v>135</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19">
       <c r="A91" t="s">
         <v>136</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19">
       <c r="A92" t="s">
         <v>137</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19">
       <c r="A93" t="s">
         <v>138</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:19">
       <c r="A94" t="s">
         <v>139</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:19">
       <c r="A95" t="s">
         <v>140</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:19">
       <c r="A96" t="s">
         <v>141</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19">
       <c r="A97" t="s">
         <v>142</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:19">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:19">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19">
       <c r="A102" t="s">
         <v>147</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19">
       <c r="A103" t="s">
         <v>148</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19">
       <c r="A104" t="s">
         <v>149</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:19">
       <c r="A105" t="s">
         <v>150</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:19">
       <c r="A106" t="s">
         <v>151</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19">
       <c r="A107" t="s">
         <v>152</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19">
       <c r="A108" t="s">
         <v>153</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:19">
       <c r="A109" t="s">
         <v>154</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:19">
       <c r="A110" t="s">
         <v>155</v>
       </c>
@@ -7603,8 +7603,8 @@
       <c r="P110">
         <v>0</v>
       </c>
-      <c r="Q110" t="s">
-        <v>24</v>
+      <c r="Q110">
+        <v>65</v>
       </c>
       <c r="R110" t="s">
         <v>22</v>
@@ -7613,7 +7613,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19">
       <c r="A111" t="s">
         <v>156</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:19">
       <c r="A112" t="s">
         <v>157</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:19">
       <c r="A113" t="s">
         <v>158</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:19">
       <c r="A114" t="s">
         <v>159</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19">
       <c r="A115" t="s">
         <v>160</v>
       </c>
@@ -7908,7 +7908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:19">
       <c r="A116" t="s">
         <v>161</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19">
       <c r="A117" t="s">
         <v>162</v>
       </c>
@@ -8016,8 +8016,8 @@
       <c r="P117">
         <v>39</v>
       </c>
-      <c r="Q117" t="s">
-        <v>24</v>
+      <c r="Q117">
+        <v>305</v>
       </c>
       <c r="R117" t="s">
         <v>22</v>
@@ -8026,7 +8026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19">
       <c r="A118" t="s">
         <v>163</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:19">
       <c r="A119" t="s">
         <v>164</v>
       </c>
@@ -8144,7 +8144,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:19">
       <c r="A120" t="s">
         <v>165</v>
       </c>
@@ -8193,8 +8193,8 @@
       <c r="P120">
         <v>2</v>
       </c>
-      <c r="Q120" t="s">
-        <v>24</v>
+      <c r="Q120">
+        <v>900</v>
       </c>
       <c r="R120" t="s">
         <v>22</v>
@@ -8203,7 +8203,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:19">
       <c r="A121" t="s">
         <v>166</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:19">
       <c r="A122" t="s">
         <v>167</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:19">
       <c r="A123" t="s">
         <v>168</v>
       </c>
@@ -8380,7 +8380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:19">
       <c r="A124" t="s">
         <v>169</v>
       </c>
@@ -8439,7 +8439,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:19">
       <c r="A125" t="s">
         <v>170</v>
       </c>
@@ -8498,7 +8498,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:19">
       <c r="A126" t="s">
         <v>171</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19">
       <c r="A127" t="s">
         <v>172</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:19">
       <c r="A128" t="s">
         <v>173</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:19">
       <c r="A129" t="s">
         <v>174</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19">
       <c r="A130" t="s">
         <v>175</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:19">
       <c r="A131" t="s">
         <v>176</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:19">
       <c r="A132" t="s">
         <v>177</v>
       </c>
@@ -8911,7 +8911,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19">
       <c r="A133" t="s">
         <v>178</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:19">
       <c r="A134" t="s">
         <v>179</v>
       </c>
@@ -9029,7 +9029,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:19">
       <c r="A135" t="s">
         <v>180</v>
       </c>
@@ -9088,7 +9088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:19">
       <c r="A136" t="s">
         <v>46</v>
       </c>
@@ -9147,7 +9147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:19">
       <c r="A137" t="s">
         <v>181</v>
       </c>
@@ -9196,8 +9196,8 @@
       <c r="P137">
         <v>18</v>
       </c>
-      <c r="Q137" t="s">
-        <v>24</v>
+      <c r="Q137">
+        <v>131.5</v>
       </c>
       <c r="R137" t="s">
         <v>20</v>
@@ -9206,7 +9206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:19">
       <c r="A138" t="s">
         <v>182</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:19">
       <c r="A139" t="s">
         <v>183</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:19">
       <c r="A140" t="s">
         <v>184</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:19">
       <c r="A141" t="s">
         <v>185</v>
       </c>
@@ -9442,7 +9442,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:19">
       <c r="A142" t="s">
         <v>186</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:19">
       <c r="A143" t="s">
         <v>187</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:19">
       <c r="A144" t="s">
         <v>188</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:19">
       <c r="A145" t="s">
         <v>189</v>
       </c>
@@ -9678,7 +9678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:19">
       <c r="A146" t="s">
         <v>190</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:19">
       <c r="A147" t="s">
         <v>191</v>
       </c>
@@ -9796,7 +9796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:19">
       <c r="A148" t="s">
         <v>192</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:19">
       <c r="A149" t="s">
         <v>193</v>
       </c>
@@ -9914,7 +9914,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:19">
       <c r="A150" t="s">
         <v>194</v>
       </c>
@@ -9973,7 +9973,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:19">
       <c r="A151" t="s">
         <v>195</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:19">
       <c r="A152" t="s">
         <v>196</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:19">
       <c r="A153" t="s">
         <v>197</v>
       </c>
@@ -10150,7 +10150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:19">
       <c r="A154" t="s">
         <v>198</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:19">
       <c r="A155" t="s">
         <v>199</v>
       </c>
@@ -10268,7 +10268,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:19">
       <c r="A156" t="s">
         <v>200</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:19">
       <c r="A157" t="s">
         <v>201</v>
       </c>
@@ -10386,7 +10386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:19">
       <c r="A158" t="s">
         <v>202</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:19">
       <c r="A159" t="s">
         <v>203</v>
       </c>
@@ -10504,7 +10504,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:19">
       <c r="A160" t="s">
         <v>204</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:19">
       <c r="A161" t="s">
         <v>205</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:19">
       <c r="A162" t="s">
         <v>206</v>
       </c>
@@ -10681,7 +10681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:19">
       <c r="A163" t="s">
         <v>207</v>
       </c>
@@ -10740,7 +10740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:19">
       <c r="A164" t="s">
         <v>208</v>
       </c>
@@ -10799,7 +10799,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:19">
       <c r="A165" t="s">
         <v>209</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:19">
       <c r="A166" t="s">
         <v>210</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:19">
       <c r="A167" t="s">
         <v>211</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:19">
       <c r="A168" t="s">
         <v>212</v>
       </c>
@@ -11035,7 +11035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:19">
       <c r="A169" t="s">
         <v>213</v>
       </c>
@@ -11094,7 +11094,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:19">
       <c r="A170" t="s">
         <v>214</v>
       </c>
@@ -11153,7 +11153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:19">
       <c r="A171" t="s">
         <v>215</v>
       </c>
@@ -11202,8 +11202,8 @@
       <c r="P171">
         <v>6</v>
       </c>
-      <c r="Q171" t="s">
-        <v>24</v>
+      <c r="Q171">
+        <v>466.71899999999999</v>
       </c>
       <c r="R171" t="s">
         <v>22</v>
@@ -11212,7 +11212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:19">
       <c r="A172" t="s">
         <v>216</v>
       </c>
@@ -11271,7 +11271,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:19">
       <c r="A173" t="s">
         <v>217</v>
       </c>
@@ -11330,7 +11330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:19">
       <c r="A174" t="s">
         <v>218</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:19">
       <c r="A175" t="s">
         <v>219</v>
       </c>
@@ -11448,7 +11448,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:19">
       <c r="A176" t="s">
         <v>220</v>
       </c>
@@ -11507,7 +11507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:19">
       <c r="A177" t="s">
         <v>221</v>
       </c>
@@ -11566,7 +11566,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:19">
       <c r="A178" t="s">
         <v>222</v>
       </c>
@@ -11625,7 +11625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:19">
       <c r="A179" t="s">
         <v>223</v>
       </c>
@@ -11684,7 +11684,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:19">
       <c r="A180" t="s">
         <v>224</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:19">
       <c r="A181" t="s">
         <v>225</v>
       </c>
@@ -11802,7 +11802,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:19">
       <c r="A182" t="s">
         <v>226</v>
       </c>
@@ -11861,7 +11861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:19">
       <c r="A183" t="s">
         <v>227</v>
       </c>
@@ -11920,7 +11920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:19">
       <c r="A184" t="s">
         <v>228</v>
       </c>
@@ -11979,7 +11979,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:19">
       <c r="A185" t="s">
         <v>229</v>
       </c>
@@ -12038,7 +12038,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:19">
       <c r="A186" t="s">
         <v>230</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:19">
       <c r="A187" t="s">
         <v>231</v>
       </c>
@@ -12156,7 +12156,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:19">
       <c r="A188" t="s">
         <v>232</v>
       </c>
@@ -12215,7 +12215,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:19">
       <c r="A189" t="s">
         <v>233</v>
       </c>
@@ -12274,7 +12274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:19">
       <c r="A190" t="s">
         <v>234</v>
       </c>
@@ -12333,7 +12333,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:19">
       <c r="A191" t="s">
         <v>235</v>
       </c>
@@ -12392,7 +12392,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:19">
       <c r="A192" t="s">
         <v>236</v>
       </c>
@@ -12451,7 +12451,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:19">
       <c r="A193" t="s">
         <v>237</v>
       </c>
@@ -12510,7 +12510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:19">
       <c r="A194" t="s">
         <v>238</v>
       </c>
@@ -12569,7 +12569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:19">
       <c r="A195" t="s">
         <v>239</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:19">
       <c r="A196" t="s">
         <v>240</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:19">
       <c r="A197" t="s">
         <v>241</v>
       </c>
@@ -12746,7 +12746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:19">
       <c r="A198" t="s">
         <v>242</v>
       </c>
@@ -12805,7 +12805,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:19">
       <c r="A199" t="s">
         <v>243</v>
       </c>
@@ -12864,7 +12864,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:19">
       <c r="A200" t="s">
         <v>244</v>
       </c>
@@ -12923,7 +12923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:19">
       <c r="A201" t="s">
         <v>245</v>
       </c>
@@ -12982,7 +12982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:19">
       <c r="A202" t="s">
         <v>246</v>
       </c>
@@ -13041,7 +13041,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:19">
       <c r="A203" t="s">
         <v>247</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:19">
       <c r="A204" t="s">
         <v>248</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:19">
       <c r="A205" t="s">
         <v>249</v>
       </c>
@@ -13218,7 +13218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:19">
       <c r="A206" t="s">
         <v>250</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:19">
       <c r="A207" t="s">
         <v>251</v>
       </c>
@@ -13338,5 +13338,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>